<commit_message>
changing to object oriented for models
</commit_message>
<xml_diff>
--- a/static/data/backtesting/output/rgb_results_[4, 8, 24, 52].xlsx
+++ b/static/data/backtesting/output/rgb_results_[4, 8, 24, 52].xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyyup\Desktop\packages\masters_thesis\static\data\backtesting\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECFF4E6-71FB-42E2-A464-502CF0AEC217}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="sheet0" sheetId="1" r:id="rId1"/>
     <sheet name="sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -134,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,14 +192,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -252,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,27 +270,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,24 +304,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -529,20 +479,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="7" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
         <v>4</v>
       </c>
@@ -556,7 +500,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,21 +511,21 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -590,24 +534,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,50 +559,50 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -675,49 +619,49 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -726,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -743,32 +687,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -777,29 +721,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -811,15 +755,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -828,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -836,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -845,46 +789,46 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -897,28 +841,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:E21">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="3Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -932,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -949,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -966,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -983,7 +918,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1000,7 +935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1017,7 +952,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +969,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1068,7 +1003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>